<commit_message>
ajout graphique et tableau
</commit_message>
<xml_diff>
--- a/INF8480 - Systèmes répartis et infonuagique/TP3/donnes.xlsx
+++ b/INF8480 - Systèmes répartis et infonuagique/TP3/donnes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Poly\H2018_1\INF8480 - Systèmes répartis et infonuagique\TP3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Poly\8-H18\INF8480 - Systèmes répartis et infonuagique\TP3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,21 +27,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>1 serveur</t>
+    <t>1 machine virtuelle</t>
   </si>
   <si>
-    <t>t1 (ms)</t>
+    <t>2 machines virtuelles avec répartiteur de charge</t>
   </si>
   <si>
-    <t>t2 (ms)</t>
+    <t>Temps1 (ms)</t>
   </si>
   <si>
-    <t>t3 (ms)</t>
+    <t>Moyenne (ms)</t>
   </si>
   <si>
-    <t>2serveurs</t>
+    <t>Temps2 (ms)</t>
+  </si>
+  <si>
+    <t>Temps3 (ms)</t>
   </si>
 </sst>
 </file>
@@ -54,15 +60,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -70,12 +82,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -91,6 +125,1325 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CA"/>
+              <a:t>Temps d'exécution selon le nombre de machines viturelles </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Temps1 (ms)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1 machine virtuelle</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 machines virtuelles avec répartiteur de charge</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$B$2:$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>25019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12927</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-920E-46EE-ABF9-991C249775D0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Temps2 (ms)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1 machine virtuelle</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 machines virtuelles avec répartiteur de charge</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$C$2:$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>24205</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11430</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-920E-46EE-ABF9-991C249775D0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Temps3 (ms)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$A$2:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1 machine virtuelle</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2 machines virtuelles avec répartiteur de charge</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$D$2:$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>23456</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11427</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-920E-46EE-ABF9-991C249775D0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="21578304"/>
+        <c:axId val="47208336"/>
+      </c:barChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Temps moyen (ms)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:softEdge rad="0"/>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="dash"/>
+            <c:size val="15"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="0" cap="sq">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:headEnd type="none" w="med" len="sm"/>
+              </a:ln>
+              <a:effectLst>
+                <a:softEdge rad="0"/>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.5175500972045446E-2"/>
+                  <c:y val="-5.8299475088829121E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-920E-46EE-ABF9-991C249775D0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.1439408474919887E-2"/>
+                  <c:y val="-4.5976902773435968E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-920E-46EE-ABF9-991C249775D0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$E$2:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>24226.666666666668</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11928</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-920E-46EE-ABF9-991C249775D0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="21578304"/>
+        <c:axId val="47208336"/>
+      </c:scatterChart>
+      <c:catAx>
+        <c:axId val="21578304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="47208336"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="47208336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA"/>
+                  <a:t>Temps d'exécution</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-CA" baseline="0"/>
+                  <a:t> (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="21578304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>551869</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>85531</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3071B17-5292-4A28-89DB-F789E9B8E29F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Temps1 (ms)</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>Temps2 (ms)</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>Temps3 (ms)</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>Temps moyen (ms)</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>2 serveurs (q₁ = 3; q₂ = 3)</v>
+          </cell>
+          <cell r="B2">
+            <v>2649.793056</v>
+          </cell>
+          <cell r="C2">
+            <v>2642.6732919999999</v>
+          </cell>
+          <cell r="D2">
+            <v>2452.9814150000002</v>
+          </cell>
+          <cell r="E2">
+            <v>2581.8159209999999</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>3 serveurs (q₁ = 3; q₂ = 3; q₃ = 4)</v>
+          </cell>
+          <cell r="B3">
+            <v>1842.510959</v>
+          </cell>
+          <cell r="C3">
+            <v>1748.6875359999999</v>
+          </cell>
+          <cell r="D3">
+            <v>1696.475232</v>
+          </cell>
+          <cell r="E3">
+            <v>1762.5579089999999</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>4 serveurs (q₁ = 3; q₂ = 3; q₃ = 3 ; q₄ = 3)</v>
+          </cell>
+          <cell r="B4">
+            <v>1418.767677</v>
+          </cell>
+          <cell r="C4">
+            <v>1360.2918299999999</v>
+          </cell>
+          <cell r="D4">
+            <v>1357.9627929999999</v>
+          </cell>
+          <cell r="E4">
+            <v>1379.0074333333332</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -390,54 +1743,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>25019</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>24205</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>23456</v>
       </c>
+      <c r="E2" s="2">
+        <f>AVERAGE(B2:D2)</f>
+        <v>24226.666666666668</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
+    <row r="3" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>12927</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>11430</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>11427</v>
+      </c>
+      <c r="E3" s="2">
+        <f>AVERAGE(B3:D3)</f>
+        <v>11928</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>